<commit_message>
ui changes for jana modules
</commit_message>
<xml_diff>
--- a/Troy.Web/Troy.Web/App_Data/ExcelFiles/Manufacturer Pre.xlsx
+++ b/Troy.Web/Troy.Web/App_Data/ExcelFiles/Manufacturer Pre.xlsx
@@ -393,7 +393,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -499,7 +499,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>105</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>

</xml_diff>